<commit_message>
import guru dan karawam
</commit_message>
<xml_diff>
--- a/public/file/format-excel-import-staff.xlsx
+++ b/public/file/format-excel-import-staff.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alfian\Documents\Projects\CoreMiSchool\public\file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ardia\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697A260E-7319-41C5-BC11-BB50EAE3BD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC274B1-9C5A-4685-9C08-E32973B3F541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>NAMA</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>Contoh Format (Jangan Dihapus)</t>
+  </si>
+  <si>
+    <t>NOMER TELEPON</t>
+  </si>
+  <si>
+    <t>0878 9878 7878</t>
   </si>
 </sst>
 </file>
@@ -405,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L999"/>
+  <dimension ref="A1:M999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -419,17 +425,17 @@
     <col min="4" max="4" width="36.88671875" customWidth="1"/>
     <col min="5" max="5" width="31.88671875" style="6" customWidth="1"/>
     <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="7" width="26.88671875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="9" width="80.6640625" customWidth="1"/>
-    <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="23.33203125" customWidth="1"/>
-    <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="28.5546875" customWidth="1"/>
-    <col min="14" max="22" width="8.6640625" customWidth="1"/>
+    <col min="7" max="8" width="26.88671875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="25" customWidth="1"/>
+    <col min="10" max="10" width="80.6640625" customWidth="1"/>
+    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="12" max="12" width="23.33203125" customWidth="1"/>
+    <col min="13" max="13" width="17" customWidth="1"/>
+    <col min="14" max="14" width="28.5546875" customWidth="1"/>
+    <col min="15" max="23" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,17 +457,20 @@
       <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:12" s="7" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="7" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
@@ -483,10 +492,13 @@
       <c r="G2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1472,13 +1484,13 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H2" xr:uid="{376A7DE1-D41A-4D0C-8AE0-24D38AD9A180}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I2" xr:uid="{376A7DE1-D41A-4D0C-8AE0-24D38AD9A180}">
       <formula1>"Islam,Kirsten,Budha,Hindu,Konghucu"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{BC52984F-D439-4617-8849-9201B3751AF4}">
       <formula1>"Laki-laki,Perempuan"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576" xr:uid="{725CF028-6837-482F-BA1B-68F565A1A17F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I1048576" xr:uid="{725CF028-6837-482F-BA1B-68F565A1A17F}">
       <formula1>"Islam,Kristen,Budha,Hindu,Konghucu"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>